<commit_message>
Update aerodynamic coefficients and enhance physics model; add next steps documentation
</commit_message>
<xml_diff>
--- a/Data_Collection/random_flightscope_data.xlsx
+++ b/Data_Collection/random_flightscope_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacksonne/Python Projects/AI_Caddie/AI_Caddie/Data_Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D14EDC6-73E2-1847-BE5A-413185D457CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A47CF66-B5B4-9940-A85F-3414E31C1570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="124">
   <si>
     <t>No.</t>
   </si>
@@ -122,6 +122,288 @@
   </si>
   <si>
     <t>Shot Classification</t>
+  </si>
+  <si>
+    <t>-26.1</t>
+  </si>
+  <si>
+    <t>-9.6</t>
+  </si>
+  <si>
+    <t>-10.7</t>
+  </si>
+  <si>
+    <t>-27.8</t>
+  </si>
+  <si>
+    <t>-1.1</t>
+  </si>
+  <si>
+    <t>-9.7</t>
+  </si>
+  <si>
+    <t>-7.8</t>
+  </si>
+  <si>
+    <t>-14.4</t>
+  </si>
+  <si>
+    <t>-7</t>
+  </si>
+  <si>
+    <t>-8.7</t>
+  </si>
+  <si>
+    <t>-7.3</t>
+  </si>
+  <si>
+    <t>-13.8</t>
+  </si>
+  <si>
+    <t>-8.1</t>
+  </si>
+  <si>
+    <t>-25.5</t>
+  </si>
+  <si>
+    <t>-10.4</t>
+  </si>
+  <si>
+    <t>-9.3</t>
+  </si>
+  <si>
+    <t>-18.4</t>
+  </si>
+  <si>
+    <t>-0.3</t>
+  </si>
+  <si>
+    <t>-16.3</t>
+  </si>
+  <si>
+    <t>-41.7</t>
+  </si>
+  <si>
+    <t>-46.4</t>
+  </si>
+  <si>
+    <t>-28</t>
+  </si>
+  <si>
+    <t>-9.2</t>
+  </si>
+  <si>
+    <t>-20.1</t>
+  </si>
+  <si>
+    <t>-9.5</t>
+  </si>
+  <si>
+    <t>-22</t>
+  </si>
+  <si>
+    <t>-10.2</t>
+  </si>
+  <si>
+    <t>-18.7</t>
+  </si>
+  <si>
+    <t>-19</t>
+  </si>
+  <si>
+    <t>-3.4</t>
+  </si>
+  <si>
+    <t>-21.6</t>
+  </si>
+  <si>
+    <t>-1.6</t>
+  </si>
+  <si>
+    <t>-9.4</t>
+  </si>
+  <si>
+    <t>-39.1</t>
+  </si>
+  <si>
+    <t>-8.8</t>
+  </si>
+  <si>
+    <t>-15.4</t>
+  </si>
+  <si>
+    <t>-43.5</t>
+  </si>
+  <si>
+    <t>-28.8</t>
+  </si>
+  <si>
+    <t>-61.5</t>
+  </si>
+  <si>
+    <t>-25.1</t>
+  </si>
+  <si>
+    <t>-14.9</t>
+  </si>
+  <si>
+    <t>-39.7</t>
+  </si>
+  <si>
+    <t>-1.8</t>
+  </si>
+  <si>
+    <t>-12.6</t>
+  </si>
+  <si>
+    <t>-18.1</t>
+  </si>
+  <si>
+    <t>-26.9</t>
+  </si>
+  <si>
+    <t>-35.5</t>
+  </si>
+  <si>
+    <t>-11</t>
+  </si>
+  <si>
+    <t>-12.5</t>
+  </si>
+  <si>
+    <t>-38.6</t>
+  </si>
+  <si>
+    <t>-41.2</t>
+  </si>
+  <si>
+    <t>-0.5</t>
+  </si>
+  <si>
+    <t>-25.4</t>
+  </si>
+  <si>
+    <t>-4.9</t>
+  </si>
+  <si>
+    <t>-26.3</t>
+  </si>
+  <si>
+    <t>-44.1</t>
+  </si>
+  <si>
+    <t>-28.5</t>
+  </si>
+  <si>
+    <t>-36.7</t>
+  </si>
+  <si>
+    <t>-15.6</t>
+  </si>
+  <si>
+    <t>-0.9</t>
+  </si>
+  <si>
+    <t>-4.8</t>
+  </si>
+  <si>
+    <t>-12</t>
+  </si>
+  <si>
+    <t>-6.5</t>
+  </si>
+  <si>
+    <t>-19.9</t>
+  </si>
+  <si>
+    <t>-13.7</t>
+  </si>
+  <si>
+    <t>-17.7</t>
+  </si>
+  <si>
+    <t>-11.7</t>
+  </si>
+  <si>
+    <t>-26.5</t>
+  </si>
+  <si>
+    <t>-6</t>
+  </si>
+  <si>
+    <t>-25.9</t>
+  </si>
+  <si>
+    <t>-19.3</t>
+  </si>
+  <si>
+    <t>-3.3</t>
+  </si>
+  <si>
+    <t>-31.9</t>
+  </si>
+  <si>
+    <t>-2.6</t>
+  </si>
+  <si>
+    <t>-12.3</t>
+  </si>
+  <si>
+    <t>-36.9</t>
+  </si>
+  <si>
+    <t>-8.6</t>
+  </si>
+  <si>
+    <t>-7.6</t>
+  </si>
+  <si>
+    <t>-30.4</t>
+  </si>
+  <si>
+    <t>-22.1</t>
+  </si>
+  <si>
+    <t>-57.9</t>
+  </si>
+  <si>
+    <t>-8</t>
+  </si>
+  <si>
+    <t>-50.5</t>
+  </si>
+  <si>
+    <t>-24</t>
+  </si>
+  <si>
+    <t>-4.3</t>
+  </si>
+  <si>
+    <t>-12.9</t>
+  </si>
+  <si>
+    <t>-6.4</t>
+  </si>
+  <si>
+    <t>-15</t>
+  </si>
+  <si>
+    <t>-2.1</t>
+  </si>
+  <si>
+    <t>-5.7</t>
+  </si>
+  <si>
+    <t>-2.9</t>
+  </si>
+  <si>
+    <t>-7.1</t>
+  </si>
+  <si>
+    <t>-1.4</t>
+  </si>
+  <si>
+    <t>-10</t>
   </si>
 </sst>
 </file>
@@ -678,23 +960,6 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -716,6 +981,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -917,7 +1199,7 @@
     </tableColumn>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Time (s)" dataDxfId="9"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Height (ft)" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{7BF7277F-7A20-5D4D-BFDD-6D4FBF3C52AA}" name="Shot Classification" dataDxfId="0">
+    <tableColumn id="26" xr3:uid="{7BF7277F-7A20-5D4D-BFDD-6D4FBF3C52AA}" name="Shot Classification" dataDxfId="7">
       <calculatedColumnFormula>IF(AND(Table1[[#This Row],[Spin Axis (deg)]]=0,Table1[[#This Row],[Launch H (deg)]]=0),"Straight",
  IF(Table1[[#This Row],[Spin Axis (deg)]]=0,
    IF(Table1[[#This Row],[Launch H (deg)]]&lt;0,"Pull",IF(Table1[[#This Row],[Launch H (deg)]]&gt;0,"Push","")),
@@ -933,13 +1215,13 @@
  )
 ))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Wind Speed (mph)" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Wind Direction (deg)" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Air Pressure (psi)" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Temperature (F)" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Humidity (%)" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Ball type" dataDxfId="2"/>
-    <tableColumn id="25" xr3:uid="{44AF1998-C229-F748-9B28-15E889997F79}" name="Altitude (ft)" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Wind Speed (mph)" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Wind Direction (deg)" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Air Pressure (psi)" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Temperature (F)" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Humidity (%)" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Ball type" dataDxfId="1"/>
+    <tableColumn id="25" xr3:uid="{44AF1998-C229-F748-9B28-15E889997F79}" name="Altitude (ft)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1245,7 +1527,7 @@
   <dimension ref="A1:Z388"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19579,15 +19861,15 @@
       <c r="I202" s="3">
         <v>5103</v>
       </c>
-      <c r="J202" s="3">
-        <v>4.3</v>
+      <c r="J202" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="K202" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L202" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="M202" s="3">
         <v>22.6</v>
@@ -19660,15 +19942,15 @@
       <c r="D203" s="3">
         <v>160.6</v>
       </c>
-      <c r="E203" s="3">
-        <v>26.1</v>
+      <c r="E203" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="F203" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G203" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-26.1</v>
+        <v>--26.1</v>
       </c>
       <c r="H203" s="3">
         <v>110</v>
@@ -19676,28 +19958,28 @@
       <c r="I203" s="3">
         <v>4482</v>
       </c>
-      <c r="J203" s="3">
-        <v>4.3</v>
+      <c r="J203" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="K203" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L203" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="M203" s="3">
         <v>19.5</v>
       </c>
-      <c r="N203" s="3">
-        <v>8.6</v>
+      <c r="N203" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O203" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P203" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q203" s="3">
         <v>5.8</v>
@@ -19757,15 +20039,15 @@
       <c r="D204" s="3">
         <v>142.30000000000001</v>
       </c>
-      <c r="E204" s="3">
-        <v>9.6</v>
+      <c r="E204" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="F204" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G204" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-9.6</v>
+        <v>--9.6</v>
       </c>
       <c r="H204" s="3">
         <v>111.4</v>
@@ -19786,15 +20068,15 @@
       <c r="M204" s="3">
         <v>24.7</v>
       </c>
-      <c r="N204" s="3">
-        <v>5.7</v>
+      <c r="N204" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="O204" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P204" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-5.7</v>
+        <v>--5.7</v>
       </c>
       <c r="Q204" s="3">
         <v>6.5</v>
@@ -19854,15 +20136,15 @@
       <c r="D205" s="3">
         <v>211.3</v>
       </c>
-      <c r="E205" s="3">
-        <v>10.7</v>
+      <c r="E205" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="F205" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G205" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-10.7</v>
+        <v>--10.7</v>
       </c>
       <c r="H205" s="3">
         <v>155.69999999999999</v>
@@ -19881,15 +20163,15 @@
       <c r="M205" s="3">
         <v>23.7</v>
       </c>
-      <c r="N205" s="3">
-        <v>2.9</v>
+      <c r="N205" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O205" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P205" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q205" s="3">
         <v>8.6999999999999993</v>
@@ -20044,15 +20326,15 @@
       <c r="D207" s="3">
         <v>226.1</v>
       </c>
-      <c r="E207" s="3">
-        <v>27.8</v>
+      <c r="E207" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F207" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G207" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-27.8</v>
+        <v>--27.8</v>
       </c>
       <c r="H207" s="3">
         <v>155.69999999999999</v>
@@ -20071,15 +20353,15 @@
       <c r="M207" s="3">
         <v>19.5</v>
       </c>
-      <c r="N207" s="3">
-        <v>7.1</v>
+      <c r="N207" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="O207" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P207" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-7.1</v>
+        <v>--7.1</v>
       </c>
       <c r="Q207" s="3">
         <v>8.3000000000000007</v>
@@ -20428,15 +20710,15 @@
       <c r="D211" s="3">
         <v>199</v>
       </c>
-      <c r="E211" s="3">
-        <v>1.1000000000000001</v>
+      <c r="E211" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="F211" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G211" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-1.1</v>
+        <v>--1.1</v>
       </c>
       <c r="H211" s="3">
         <v>140</v>
@@ -20444,15 +20726,15 @@
       <c r="I211" s="3">
         <v>4689</v>
       </c>
-      <c r="J211" s="3">
-        <v>10.7</v>
+      <c r="J211" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K211" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L211" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-10.7</v>
+        <v>--10.7</v>
       </c>
       <c r="M211" s="3">
         <v>28.9</v>
@@ -20620,15 +20902,15 @@
       <c r="D213" s="3">
         <v>157.9</v>
       </c>
-      <c r="E213" s="3">
-        <v>9.6999999999999993</v>
+      <c r="E213" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="F213" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G213" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-9.7</v>
+        <v>--9.7</v>
       </c>
       <c r="H213" s="3">
         <v>115.7</v>
@@ -20636,15 +20918,15 @@
       <c r="I213" s="3">
         <v>5517</v>
       </c>
-      <c r="J213" s="3">
-        <v>12.9</v>
+      <c r="J213" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="K213" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L213" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-12.9</v>
+        <v>--12.9</v>
       </c>
       <c r="M213" s="3">
         <v>27.9</v>
@@ -20715,15 +20997,15 @@
       <c r="D214" s="3">
         <v>164.1</v>
       </c>
-      <c r="E214" s="3">
-        <v>7.8</v>
+      <c r="E214" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F214" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G214" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-7.8</v>
+        <v>--7.8</v>
       </c>
       <c r="H214" s="3">
         <v>112.9</v>
@@ -20731,28 +21013,28 @@
       <c r="I214" s="3">
         <v>4689</v>
       </c>
-      <c r="J214" s="3">
-        <v>6.4</v>
+      <c r="J214" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K214" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L214" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M214" s="3">
         <v>15.3</v>
       </c>
-      <c r="N214" s="3">
-        <v>1.4</v>
+      <c r="N214" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O214" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P214" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q214" s="3">
         <v>5.5</v>
@@ -20812,15 +21094,15 @@
       <c r="D215" s="3">
         <v>273.2</v>
       </c>
-      <c r="E215" s="3">
-        <v>14.4</v>
+      <c r="E215" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="F215" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G215" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-14.4</v>
+        <v>--14.4</v>
       </c>
       <c r="H215" s="3">
         <v>164.3</v>
@@ -20828,28 +21110,28 @@
       <c r="I215" s="3">
         <v>2827</v>
       </c>
-      <c r="J215" s="3">
-        <v>6.4</v>
+      <c r="J215" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K215" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L215" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M215" s="3">
         <v>21.6</v>
       </c>
-      <c r="N215" s="3">
-        <v>1.4</v>
+      <c r="N215" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O215" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P215" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q215" s="3">
         <v>8.5</v>
@@ -21101,15 +21383,15 @@
       <c r="D218" s="3">
         <v>272.3</v>
       </c>
-      <c r="E218" s="3">
-        <v>7</v>
+      <c r="E218" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="F218" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G218" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-7</v>
+        <v>--7</v>
       </c>
       <c r="H218" s="3">
         <v>162.9</v>
@@ -21130,15 +21412,15 @@
       <c r="M218" s="3">
         <v>11.1</v>
       </c>
-      <c r="N218" s="3">
-        <v>4.3</v>
+      <c r="N218" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O218" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P218" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q218" s="3">
         <v>6.7</v>
@@ -21214,15 +21496,15 @@
       <c r="I219" s="3">
         <v>4896</v>
       </c>
-      <c r="J219" s="3">
-        <v>10.7</v>
+      <c r="J219" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K219" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L219" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-10.7</v>
+        <v>--10.7</v>
       </c>
       <c r="M219" s="3">
         <v>17.399999999999999</v>
@@ -21392,15 +21674,15 @@
       <c r="D221" s="3">
         <v>161.19999999999999</v>
       </c>
-      <c r="E221" s="3">
-        <v>8.6999999999999993</v>
+      <c r="E221" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="F221" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G221" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-8.7</v>
+        <v>--8.7</v>
       </c>
       <c r="H221" s="3">
         <v>120</v>
@@ -21408,15 +21690,15 @@
       <c r="I221" s="3">
         <v>5931</v>
       </c>
-      <c r="J221" s="3">
-        <v>10.7</v>
+      <c r="J221" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K221" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L221" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-10.7</v>
+        <v>--10.7</v>
       </c>
       <c r="M221" s="3">
         <v>27.9</v>
@@ -21584,15 +21866,15 @@
       <c r="D223" s="3">
         <v>269.60000000000002</v>
       </c>
-      <c r="E223" s="3">
-        <v>7.3</v>
+      <c r="E223" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="F223" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G223" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-7.3</v>
+        <v>--7.3</v>
       </c>
       <c r="H223" s="3">
         <v>177.1</v>
@@ -21613,15 +21895,15 @@
       <c r="M223" s="3">
         <v>11.1</v>
       </c>
-      <c r="N223" s="3">
-        <v>2.9</v>
+      <c r="N223" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O223" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P223" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q223" s="3">
         <v>8.1</v>
@@ -21697,15 +21979,15 @@
       <c r="I224" s="3">
         <v>3655</v>
       </c>
-      <c r="J224" s="3">
-        <v>4.3</v>
+      <c r="J224" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="K224" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L224" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="M224" s="3">
         <v>21.6</v>
@@ -21778,15 +22060,15 @@
       <c r="D225" s="3">
         <v>208</v>
       </c>
-      <c r="E225" s="3">
-        <v>13.8</v>
+      <c r="E225" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="F225" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G225" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-13.8</v>
+        <v>--13.8</v>
       </c>
       <c r="H225" s="3">
         <v>158.6</v>
@@ -21794,15 +22076,15 @@
       <c r="I225" s="3">
         <v>6758</v>
       </c>
-      <c r="J225" s="3">
-        <v>10.7</v>
+      <c r="J225" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K225" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L225" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-10.7</v>
+        <v>--10.7</v>
       </c>
       <c r="M225" s="3">
         <v>27.9</v>
@@ -21968,15 +22250,15 @@
       <c r="D227" s="3">
         <v>196.4</v>
       </c>
-      <c r="E227" s="3">
-        <v>8.1</v>
+      <c r="E227" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="F227" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G227" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-8.1</v>
+        <v>--8.1</v>
       </c>
       <c r="H227" s="3">
         <v>125.7</v>
@@ -21997,15 +22279,15 @@
       <c r="M227" s="3">
         <v>13.2</v>
       </c>
-      <c r="N227" s="3">
-        <v>2.9</v>
+      <c r="N227" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O227" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P227" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q227" s="3">
         <v>5.6</v>
@@ -22081,15 +22363,15 @@
       <c r="I228" s="3">
         <v>6344</v>
       </c>
-      <c r="J228" s="3">
-        <v>15</v>
+      <c r="J228" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="K228" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L228" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-15</v>
+        <v>--15</v>
       </c>
       <c r="M228" s="3">
         <v>30</v>
@@ -22275,15 +22557,15 @@
       <c r="I230" s="3">
         <v>5724</v>
       </c>
-      <c r="J230" s="3">
-        <v>2.1</v>
+      <c r="J230" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="K230" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L230" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-2.1</v>
+        <v>--2.1</v>
       </c>
       <c r="M230" s="3">
         <v>19.5</v>
@@ -22356,15 +22638,15 @@
       <c r="D231" s="3">
         <v>146.6</v>
       </c>
-      <c r="E231" s="3">
-        <v>25.5</v>
+      <c r="E231" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="F231" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G231" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-25.5</v>
+        <v>--25.5</v>
       </c>
       <c r="H231" s="3">
         <v>118.6</v>
@@ -22383,15 +22665,15 @@
       <c r="M231" s="3">
         <v>30</v>
       </c>
-      <c r="N231" s="3">
-        <v>10</v>
+      <c r="N231" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O231" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P231" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q231" s="3">
         <v>7.2</v>
@@ -22548,15 +22830,15 @@
       <c r="D233" s="3">
         <v>149.1</v>
       </c>
-      <c r="E233" s="3">
-        <v>10.4</v>
+      <c r="E233" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="F233" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G233" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-10.4</v>
+        <v>--10.4</v>
       </c>
       <c r="H233" s="3">
         <v>114.3</v>
@@ -22577,15 +22859,15 @@
       <c r="M233" s="3">
         <v>28.9</v>
       </c>
-      <c r="N233" s="3">
-        <v>7.1</v>
+      <c r="N233" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="O233" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P233" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-7.1</v>
+        <v>--7.1</v>
       </c>
       <c r="Q233" s="3">
         <v>6.9</v>
@@ -22661,15 +22943,15 @@
       <c r="I234" s="3">
         <v>5724</v>
       </c>
-      <c r="J234" s="3">
-        <v>2.1</v>
+      <c r="J234" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="K234" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L234" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-2.1</v>
+        <v>--2.1</v>
       </c>
       <c r="M234" s="3">
         <v>19.5</v>
@@ -22742,15 +23024,15 @@
       <c r="D235" s="3">
         <v>238.5</v>
       </c>
-      <c r="E235" s="3">
-        <v>9.3000000000000007</v>
+      <c r="E235" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="F235" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G235" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-9.3</v>
+        <v>--9.3</v>
       </c>
       <c r="H235" s="3">
         <v>162.9</v>
@@ -22771,15 +23053,15 @@
       <c r="M235" s="3">
         <v>23.7</v>
       </c>
-      <c r="N235" s="3">
-        <v>5.7</v>
+      <c r="N235" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="O235" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P235" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-5.7</v>
+        <v>--5.7</v>
       </c>
       <c r="Q235" s="3">
         <v>8.9</v>
@@ -22936,15 +23218,15 @@
       <c r="D237" s="3">
         <v>213.3</v>
       </c>
-      <c r="E237" s="3">
-        <v>18.399999999999999</v>
+      <c r="E237" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="F237" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G237" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-18.4</v>
+        <v>--18.4</v>
       </c>
       <c r="H237" s="3">
         <v>157.1</v>
@@ -22965,15 +23247,15 @@
       <c r="M237" s="3">
         <v>28.9</v>
       </c>
-      <c r="N237" s="3">
-        <v>8.6</v>
+      <c r="N237" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O237" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P237" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q237" s="3">
         <v>9.1</v>
@@ -23128,15 +23410,15 @@
       <c r="D239" s="3">
         <v>161.5</v>
       </c>
-      <c r="E239" s="3">
-        <v>0.3</v>
+      <c r="E239" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="F239" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G239" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-0.3</v>
+        <v>--0.3</v>
       </c>
       <c r="H239" s="3">
         <v>114.3</v>
@@ -23157,15 +23439,15 @@
       <c r="M239" s="3">
         <v>10</v>
       </c>
-      <c r="N239" s="3">
-        <v>1.4</v>
+      <c r="N239" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O239" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P239" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q239" s="3">
         <v>4.7</v>
@@ -23225,15 +23507,15 @@
       <c r="D240" s="3">
         <v>163.6</v>
       </c>
-      <c r="E240" s="3">
-        <v>16.3</v>
+      <c r="E240" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="F240" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G240" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-16.3</v>
+        <v>--16.3</v>
       </c>
       <c r="H240" s="3">
         <v>132.9</v>
@@ -23252,15 +23534,15 @@
       <c r="M240" s="3">
         <v>28.9</v>
       </c>
-      <c r="N240" s="3">
-        <v>5.7</v>
+      <c r="N240" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="O240" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P240" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-5.7</v>
+        <v>--5.7</v>
       </c>
       <c r="Q240" s="3">
         <v>7.9</v>
@@ -23320,15 +23602,15 @@
       <c r="D241" s="3">
         <v>256.8</v>
       </c>
-      <c r="E241" s="3">
-        <v>41.7</v>
+      <c r="E241" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="F241" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G241" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-41.7</v>
+        <v>--41.7</v>
       </c>
       <c r="H241" s="3">
         <v>161.4</v>
@@ -23349,15 +23631,15 @@
       <c r="M241" s="3">
         <v>27.9</v>
       </c>
-      <c r="N241" s="3">
-        <v>10</v>
+      <c r="N241" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O241" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P241" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q241" s="3">
         <v>9.1</v>
@@ -23815,15 +24097,15 @@
       <c r="I246" s="3">
         <v>5103</v>
       </c>
-      <c r="J246" s="3">
-        <v>2.1</v>
+      <c r="J246" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="K246" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L246" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-2.1</v>
+        <v>--2.1</v>
       </c>
       <c r="M246" s="3">
         <v>21.6</v>
@@ -23896,15 +24178,15 @@
       <c r="D247" s="3">
         <v>239.9</v>
       </c>
-      <c r="E247" s="3">
-        <v>46.4</v>
+      <c r="E247" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="F247" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G247" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-46.4</v>
+        <v>--46.4</v>
       </c>
       <c r="H247" s="3">
         <v>161.4</v>
@@ -23912,28 +24194,28 @@
       <c r="I247" s="3">
         <v>6551</v>
       </c>
-      <c r="J247" s="3">
-        <v>8.6</v>
+      <c r="J247" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="K247" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L247" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="M247" s="3">
         <v>11.1</v>
       </c>
-      <c r="N247" s="3">
-        <v>8.6</v>
+      <c r="N247" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O247" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P247" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q247" s="3">
         <v>7.5</v>
@@ -24106,15 +24388,15 @@
       <c r="I249" s="3">
         <v>2206</v>
       </c>
-      <c r="J249" s="3">
-        <v>6.4</v>
+      <c r="J249" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K249" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L249" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M249" s="3">
         <v>27.9</v>
@@ -24470,15 +24752,15 @@
       <c r="D253" s="3">
         <v>239</v>
       </c>
-      <c r="E253" s="3">
-        <v>28</v>
+      <c r="E253" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="F253" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G253" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-28</v>
+        <v>--28</v>
       </c>
       <c r="H253" s="3">
         <v>148.6</v>
@@ -24499,15 +24781,15 @@
       <c r="M253" s="3">
         <v>12.1</v>
       </c>
-      <c r="N253" s="3">
-        <v>10</v>
+      <c r="N253" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O253" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P253" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q253" s="3">
         <v>6.6</v>
@@ -24583,15 +24865,15 @@
       <c r="I254" s="3">
         <v>6137</v>
       </c>
-      <c r="J254" s="3">
-        <v>10.7</v>
+      <c r="J254" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K254" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L254" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-10.7</v>
+        <v>--10.7</v>
       </c>
       <c r="M254" s="3">
         <v>28.9</v>
@@ -24693,15 +24975,15 @@
       <c r="M255" s="3">
         <v>23.7</v>
       </c>
-      <c r="N255" s="3">
-        <v>2.9</v>
+      <c r="N255" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O255" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P255" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q255" s="3">
         <v>6.7</v>
@@ -24761,15 +25043,15 @@
       <c r="D256" s="3">
         <v>182.7</v>
       </c>
-      <c r="E256" s="3">
-        <v>9.1999999999999993</v>
+      <c r="E256" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="F256" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G256" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-9.2</v>
+        <v>--9.2</v>
       </c>
       <c r="H256" s="3">
         <v>142.9</v>
@@ -24788,15 +25070,15 @@
       <c r="M256" s="3">
         <v>27.9</v>
       </c>
-      <c r="N256" s="3">
-        <v>2.9</v>
+      <c r="N256" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O256" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P256" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q256" s="3">
         <v>8.4</v>
@@ -24856,15 +25138,15 @@
       <c r="D257" s="3">
         <v>165</v>
       </c>
-      <c r="E257" s="3">
-        <v>20.100000000000001</v>
+      <c r="E257" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="F257" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G257" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-20.1</v>
+        <v>--20.1</v>
       </c>
       <c r="H257" s="3">
         <v>111.4</v>
@@ -24872,28 +25154,28 @@
       <c r="I257" s="3">
         <v>4068</v>
       </c>
-      <c r="J257" s="3">
-        <v>6.4</v>
+      <c r="J257" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K257" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L257" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M257" s="3">
         <v>22.6</v>
       </c>
-      <c r="N257" s="3">
-        <v>5.7</v>
+      <c r="N257" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="O257" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P257" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-5.7</v>
+        <v>--5.7</v>
       </c>
       <c r="Q257" s="3">
         <v>6.1</v>
@@ -25048,15 +25330,15 @@
       <c r="D259" s="3">
         <v>276.3</v>
       </c>
-      <c r="E259" s="3">
-        <v>9.5</v>
+      <c r="E259" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="F259" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G259" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-9.5</v>
+        <v>--9.5</v>
       </c>
       <c r="H259" s="3">
         <v>172.9</v>
@@ -25064,28 +25346,28 @@
       <c r="I259" s="3">
         <v>3241</v>
       </c>
-      <c r="J259" s="3">
-        <v>2.1</v>
+      <c r="J259" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="K259" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L259" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-2.1</v>
+        <v>--2.1</v>
       </c>
       <c r="M259" s="3">
         <v>24.7</v>
       </c>
-      <c r="N259" s="3">
-        <v>1.4</v>
+      <c r="N259" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O259" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P259" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q259" s="3">
         <v>9.4</v>
@@ -25240,15 +25522,15 @@
       <c r="D261" s="3">
         <v>225.6</v>
       </c>
-      <c r="E261" s="3">
-        <v>22</v>
+      <c r="E261" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="F261" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G261" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-22</v>
+        <v>--22</v>
       </c>
       <c r="H261" s="3">
         <v>155.69999999999999</v>
@@ -25256,28 +25538,28 @@
       <c r="I261" s="3">
         <v>7172</v>
       </c>
-      <c r="J261" s="3">
-        <v>4.3</v>
+      <c r="J261" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="K261" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L261" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="M261" s="3">
         <v>10</v>
       </c>
-      <c r="N261" s="3">
-        <v>4.3</v>
+      <c r="N261" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O261" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P261" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q261" s="3">
         <v>7.2</v>
@@ -25434,15 +25716,15 @@
       <c r="D263" s="3">
         <v>201.5</v>
       </c>
-      <c r="E263" s="3">
-        <v>10.199999999999999</v>
+      <c r="E263" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="F263" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G263" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-10.2</v>
+        <v>--10.2</v>
       </c>
       <c r="H263" s="3">
         <v>134.30000000000001</v>
@@ -25463,15 +25745,15 @@
       <c r="M263" s="3">
         <v>12.1</v>
       </c>
-      <c r="N263" s="3">
-        <v>5.7</v>
+      <c r="N263" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="O263" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P263" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-5.7</v>
+        <v>--5.7</v>
       </c>
       <c r="Q263" s="3">
         <v>6.2</v>
@@ -25547,15 +25829,15 @@
       <c r="I264" s="3">
         <v>2413</v>
       </c>
-      <c r="J264" s="3">
-        <v>6.4</v>
+      <c r="J264" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K264" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L264" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M264" s="3">
         <v>22.6</v>
@@ -25628,15 +25910,15 @@
       <c r="D265" s="3">
         <v>245.8</v>
       </c>
-      <c r="E265" s="3">
-        <v>18.7</v>
+      <c r="E265" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="F265" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G265" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-18.7</v>
+        <v>--18.7</v>
       </c>
       <c r="H265" s="3">
         <v>172.9</v>
@@ -25644,28 +25926,28 @@
       <c r="I265" s="3">
         <v>7172</v>
       </c>
-      <c r="J265" s="3">
-        <v>8.6</v>
+      <c r="J265" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="K265" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L265" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="M265" s="3">
         <v>18.399999999999999</v>
       </c>
-      <c r="N265" s="3">
-        <v>1.4</v>
+      <c r="N265" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O265" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P265" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q265" s="3">
         <v>8.9</v>
@@ -25741,15 +26023,15 @@
       <c r="I266" s="3">
         <v>3862</v>
       </c>
-      <c r="J266" s="3">
-        <v>4.3</v>
+      <c r="J266" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="K266" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L266" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="M266" s="3">
         <v>21.6</v>
@@ -25822,15 +26104,15 @@
       <c r="D267" s="3">
         <v>225.2</v>
       </c>
-      <c r="E267" s="3">
-        <v>19</v>
+      <c r="E267" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="F267" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G267" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-19</v>
+        <v>--19</v>
       </c>
       <c r="H267" s="3">
         <v>155.69999999999999</v>
@@ -25838,15 +26120,15 @@
       <c r="I267" s="3">
         <v>6965</v>
       </c>
-      <c r="J267" s="3">
-        <v>15</v>
+      <c r="J267" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="K267" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L267" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-15</v>
+        <v>--15</v>
       </c>
       <c r="M267" s="3">
         <v>15.3</v>
@@ -25917,15 +26199,15 @@
       <c r="D268" s="3">
         <v>229.3</v>
       </c>
-      <c r="E268" s="3">
-        <v>3.4</v>
+      <c r="E268" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="F268" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G268" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-3.4</v>
+        <v>--3.4</v>
       </c>
       <c r="H268" s="3">
         <v>140</v>
@@ -25946,15 +26228,15 @@
       <c r="M268" s="3">
         <v>19.5</v>
       </c>
-      <c r="N268" s="3">
-        <v>2.9</v>
+      <c r="N268" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O268" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P268" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q268" s="3">
         <v>7.2</v>
@@ -26014,15 +26296,15 @@
       <c r="D269" s="3">
         <v>222.3</v>
       </c>
-      <c r="E269" s="3">
-        <v>21.6</v>
+      <c r="E269" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="F269" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G269" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-21.6</v>
+        <v>--21.6</v>
       </c>
       <c r="H269" s="3">
         <v>158.6</v>
@@ -26043,15 +26325,15 @@
       <c r="M269" s="3">
         <v>16.3</v>
       </c>
-      <c r="N269" s="3">
-        <v>10</v>
+      <c r="N269" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O269" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P269" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q269" s="3">
         <v>8.1</v>
@@ -26111,15 +26393,15 @@
       <c r="D270" s="3">
         <v>193.3</v>
       </c>
-      <c r="E270" s="3">
-        <v>1.6</v>
+      <c r="E270" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="F270" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G270" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-1.6</v>
+        <v>--1.6</v>
       </c>
       <c r="H270" s="3">
         <v>127.1</v>
@@ -26140,15 +26422,15 @@
       <c r="M270" s="3">
         <v>11.1</v>
       </c>
-      <c r="N270" s="3">
-        <v>1.4</v>
+      <c r="N270" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O270" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P270" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q270" s="3">
         <v>5.5</v>
@@ -26208,15 +26490,15 @@
       <c r="D271" s="3">
         <v>171.6</v>
       </c>
-      <c r="E271" s="3">
-        <v>10.7</v>
+      <c r="E271" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="F271" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G271" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-10.7</v>
+        <v>--10.7</v>
       </c>
       <c r="H271" s="3">
         <v>115.7</v>
@@ -26237,15 +26519,15 @@
       <c r="M271" s="3">
         <v>22.6</v>
       </c>
-      <c r="N271" s="3">
-        <v>5.7</v>
+      <c r="N271" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="O271" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P271" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-5.7</v>
+        <v>--5.7</v>
       </c>
       <c r="Q271" s="3">
         <v>6.4</v>
@@ -26321,15 +26603,15 @@
       <c r="I272" s="3">
         <v>4275</v>
       </c>
-      <c r="J272" s="3">
-        <v>12.9</v>
+      <c r="J272" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="K272" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L272" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-12.9</v>
+        <v>--12.9</v>
       </c>
       <c r="M272" s="3">
         <v>12.1</v>
@@ -26418,15 +26700,15 @@
       <c r="I273" s="3">
         <v>8000</v>
       </c>
-      <c r="J273" s="3">
-        <v>8.6</v>
+      <c r="J273" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="K273" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L273" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="M273" s="3">
         <v>13.2</v>
@@ -26499,15 +26781,15 @@
       <c r="D274" s="3">
         <v>267.2</v>
       </c>
-      <c r="E274" s="3">
-        <v>9.4</v>
+      <c r="E274" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="F274" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G274" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-9.4</v>
+        <v>--9.4</v>
       </c>
       <c r="H274" s="3">
         <v>172.9</v>
@@ -26515,28 +26797,28 @@
       <c r="I274" s="3">
         <v>5310</v>
       </c>
-      <c r="J274" s="3">
-        <v>2.1</v>
+      <c r="J274" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="K274" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L274" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-2.1</v>
+        <v>--2.1</v>
       </c>
       <c r="M274" s="3">
         <v>15.3</v>
       </c>
-      <c r="N274" s="3">
-        <v>1.4</v>
+      <c r="N274" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O274" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P274" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q274" s="3">
         <v>8.5</v>
@@ -26788,15 +27070,15 @@
       <c r="D277" s="3">
         <v>206.2</v>
       </c>
-      <c r="E277" s="3">
-        <v>39.1</v>
+      <c r="E277" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="F277" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G277" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-39.1</v>
+        <v>--39.1</v>
       </c>
       <c r="H277" s="3">
         <v>125.7</v>
@@ -26804,28 +27086,28 @@
       <c r="I277" s="3">
         <v>2413</v>
       </c>
-      <c r="J277" s="3">
-        <v>12.9</v>
+      <c r="J277" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="K277" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L277" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-12.9</v>
+        <v>--12.9</v>
       </c>
       <c r="M277" s="3">
         <v>22.6</v>
       </c>
-      <c r="N277" s="3">
-        <v>8.6</v>
+      <c r="N277" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O277" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P277" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q277" s="3">
         <v>6.7</v>
@@ -26885,15 +27167,15 @@
       <c r="D278" s="3">
         <v>158.69999999999999</v>
       </c>
-      <c r="E278" s="3">
-        <v>8.8000000000000007</v>
+      <c r="E278" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="F278" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G278" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-8.8</v>
+        <v>--8.8</v>
       </c>
       <c r="H278" s="3">
         <v>110</v>
@@ -26901,28 +27183,28 @@
       <c r="I278" s="3">
         <v>3862</v>
       </c>
-      <c r="J278" s="3">
-        <v>10.7</v>
+      <c r="J278" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K278" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L278" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-10.7</v>
+        <v>--10.7</v>
       </c>
       <c r="M278" s="3">
         <v>12.1</v>
       </c>
-      <c r="N278" s="3">
-        <v>1.4</v>
+      <c r="N278" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O278" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P278" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q278" s="3">
         <v>4.5999999999999996</v>
@@ -26982,15 +27264,15 @@
       <c r="D279" s="3">
         <v>202.5</v>
       </c>
-      <c r="E279" s="3">
-        <v>15.4</v>
+      <c r="E279" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="F279" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G279" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-15.4</v>
+        <v>--15.4</v>
       </c>
       <c r="H279" s="3">
         <v>140</v>
@@ -27011,15 +27293,15 @@
       <c r="M279" s="3">
         <v>23.7</v>
       </c>
-      <c r="N279" s="3">
-        <v>5.7</v>
+      <c r="N279" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="O279" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P279" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-5.7</v>
+        <v>--5.7</v>
       </c>
       <c r="Q279" s="3">
         <v>7.9</v>
@@ -27079,15 +27361,15 @@
       <c r="D280" s="3">
         <v>254.4</v>
       </c>
-      <c r="E280" s="3">
-        <v>43.5</v>
+      <c r="E280" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="F280" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G280" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-43.5</v>
+        <v>--43.5</v>
       </c>
       <c r="H280" s="3">
         <v>161.4</v>
@@ -27106,15 +27388,15 @@
       <c r="M280" s="3">
         <v>11.1</v>
       </c>
-      <c r="N280" s="3">
-        <v>10</v>
+      <c r="N280" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O280" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P280" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q280" s="3">
         <v>7.3</v>
@@ -27203,15 +27485,15 @@
       <c r="M281" s="3">
         <v>28.9</v>
       </c>
-      <c r="N281" s="3">
-        <v>4.3</v>
+      <c r="N281" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O281" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P281" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q281" s="3">
         <v>9.4</v>
@@ -27366,15 +27648,15 @@
       <c r="D283" s="3">
         <v>205.4</v>
       </c>
-      <c r="E283" s="3">
-        <v>10.4</v>
+      <c r="E283" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="F283" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G283" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-10.4</v>
+        <v>--10.4</v>
       </c>
       <c r="H283" s="3">
         <v>164.3</v>
@@ -27393,15 +27675,15 @@
       <c r="M283" s="3">
         <v>30</v>
       </c>
-      <c r="N283" s="3">
-        <v>2.9</v>
+      <c r="N283" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O283" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P283" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q283" s="3">
         <v>9.5</v>
@@ -27461,15 +27743,15 @@
       <c r="D284" s="3">
         <v>241.5</v>
       </c>
-      <c r="E284" s="3">
-        <v>28.8</v>
+      <c r="E284" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="F284" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G284" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-28.8</v>
+        <v>--28.8</v>
       </c>
       <c r="H284" s="3">
         <v>158.6</v>
@@ -27477,28 +27759,28 @@
       <c r="I284" s="3">
         <v>5310</v>
       </c>
-      <c r="J284" s="3">
-        <v>8.6</v>
+      <c r="J284" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="K284" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L284" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="M284" s="3">
         <v>17.399999999999999</v>
       </c>
-      <c r="N284" s="3">
-        <v>4.3</v>
+      <c r="N284" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O284" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P284" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q284" s="3">
         <v>8.1</v>
@@ -27558,15 +27840,15 @@
       <c r="D285" s="3">
         <v>277.3</v>
       </c>
-      <c r="E285" s="3">
-        <v>61.5</v>
+      <c r="E285" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="F285" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G285" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-61.5</v>
+        <v>--61.5</v>
       </c>
       <c r="H285" s="3">
         <v>168.6</v>
@@ -27574,28 +27856,28 @@
       <c r="I285" s="3">
         <v>3448</v>
       </c>
-      <c r="J285" s="3">
-        <v>12.9</v>
+      <c r="J285" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="K285" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L285" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-12.9</v>
+        <v>--12.9</v>
       </c>
       <c r="M285" s="3">
         <v>11.1</v>
       </c>
-      <c r="N285" s="3">
-        <v>10</v>
+      <c r="N285" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O285" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P285" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q285" s="3">
         <v>7.2</v>
@@ -27684,15 +27966,15 @@
       <c r="M286" s="3">
         <v>26.8</v>
       </c>
-      <c r="N286" s="3">
-        <v>1.4</v>
+      <c r="N286" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O286" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P286" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q286" s="3">
         <v>8.1</v>
@@ -27752,15 +28034,15 @@
       <c r="D287" s="3">
         <v>176</v>
       </c>
-      <c r="E287" s="3">
-        <v>25.1</v>
+      <c r="E287" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="F287" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G287" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-25.1</v>
+        <v>--25.1</v>
       </c>
       <c r="H287" s="3">
         <v>111.4</v>
@@ -27779,15 +28061,15 @@
       <c r="M287" s="3">
         <v>19.5</v>
       </c>
-      <c r="N287" s="3">
-        <v>8.6</v>
+      <c r="N287" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O287" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P287" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q287" s="3">
         <v>5.5</v>
@@ -27847,15 +28129,15 @@
       <c r="D288" s="3">
         <v>245.4</v>
       </c>
-      <c r="E288" s="3">
-        <v>14.9</v>
+      <c r="E288" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="F288" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G288" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-14.9</v>
+        <v>--14.9</v>
       </c>
       <c r="H288" s="3">
         <v>147.1</v>
@@ -27863,15 +28145,15 @@
       <c r="I288" s="3">
         <v>2206</v>
       </c>
-      <c r="J288" s="3">
-        <v>15</v>
+      <c r="J288" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="K288" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L288" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-15</v>
+        <v>--15</v>
       </c>
       <c r="M288" s="3">
         <v>25.8</v>
@@ -27958,15 +28240,15 @@
       <c r="I289" s="3">
         <v>5931</v>
       </c>
-      <c r="J289" s="3">
-        <v>8.6</v>
+      <c r="J289" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="K289" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L289" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="M289" s="3">
         <v>11.1</v>
@@ -28039,15 +28321,15 @@
       <c r="D290" s="3">
         <v>298.39999999999998</v>
       </c>
-      <c r="E290" s="3">
-        <v>39.700000000000003</v>
+      <c r="E290" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="F290" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G290" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-39.7</v>
+        <v>--39.7</v>
       </c>
       <c r="H290" s="3">
         <v>178.6</v>
@@ -28068,15 +28350,15 @@
       <c r="M290" s="3">
         <v>14.2</v>
       </c>
-      <c r="N290" s="3">
-        <v>10</v>
+      <c r="N290" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O290" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P290" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q290" s="3">
         <v>8.1</v>
@@ -28136,15 +28418,15 @@
       <c r="D291" s="3">
         <v>184.7</v>
       </c>
-      <c r="E291" s="3">
-        <v>1.8</v>
+      <c r="E291" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="F291" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G291" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-1.8</v>
+        <v>--1.8</v>
       </c>
       <c r="H291" s="3">
         <v>137.1</v>
@@ -28152,15 +28434,15 @@
       <c r="I291" s="3">
         <v>6344</v>
       </c>
-      <c r="J291" s="3">
-        <v>15</v>
+      <c r="J291" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="K291" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L291" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-15</v>
+        <v>--15</v>
       </c>
       <c r="M291" s="3">
         <v>26.8</v>
@@ -28328,15 +28610,15 @@
       <c r="D293" s="3">
         <v>192.9</v>
       </c>
-      <c r="E293" s="3">
-        <v>12.6</v>
+      <c r="E293" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="F293" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G293" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-12.6</v>
+        <v>--12.6</v>
       </c>
       <c r="H293" s="3">
         <v>124.3</v>
@@ -28357,15 +28639,15 @@
       <c r="M293" s="3">
         <v>28.9</v>
       </c>
-      <c r="N293" s="3">
-        <v>4.3</v>
+      <c r="N293" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O293" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P293" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q293" s="3">
         <v>7.4</v>
@@ -28522,15 +28804,15 @@
       <c r="D295" s="3">
         <v>166.4</v>
       </c>
-      <c r="E295" s="3">
-        <v>18.100000000000001</v>
+      <c r="E295" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="F295" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G295" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-18.1</v>
+        <v>--18.1</v>
       </c>
       <c r="H295" s="3">
         <v>110</v>
@@ -28538,28 +28820,28 @@
       <c r="I295" s="3">
         <v>2620</v>
       </c>
-      <c r="J295" s="3">
-        <v>6.4</v>
+      <c r="J295" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K295" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L295" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M295" s="3">
         <v>14.2</v>
       </c>
-      <c r="N295" s="3">
-        <v>5.7</v>
+      <c r="N295" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="O295" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P295" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-5.7</v>
+        <v>--5.7</v>
       </c>
       <c r="Q295" s="3">
         <v>4.5999999999999996</v>
@@ -28619,15 +28901,15 @@
       <c r="D296" s="3">
         <v>158.1</v>
       </c>
-      <c r="E296" s="3">
-        <v>26.9</v>
+      <c r="E296" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="F296" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G296" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-26.9</v>
+        <v>--26.9</v>
       </c>
       <c r="H296" s="3">
         <v>114.3</v>
@@ -28635,28 +28917,28 @@
       <c r="I296" s="3">
         <v>5931</v>
       </c>
-      <c r="J296" s="3">
-        <v>6.4</v>
+      <c r="J296" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K296" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L296" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M296" s="3">
         <v>11.1</v>
       </c>
-      <c r="N296" s="3">
-        <v>8.6</v>
+      <c r="N296" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O296" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P296" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q296" s="3">
         <v>5.0999999999999996</v>
@@ -28716,15 +28998,15 @@
       <c r="D297" s="3">
         <v>240.2</v>
       </c>
-      <c r="E297" s="3">
-        <v>35.5</v>
+      <c r="E297" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="F297" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G297" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-35.5</v>
+        <v>--35.5</v>
       </c>
       <c r="H297" s="3">
         <v>157.1</v>
@@ -28743,15 +29025,15 @@
       <c r="M297" s="3">
         <v>12.1</v>
       </c>
-      <c r="N297" s="3">
-        <v>8.6</v>
+      <c r="N297" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O297" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P297" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q297" s="3">
         <v>7.4</v>
@@ -28922,15 +29204,15 @@
       <c r="I299" s="3">
         <v>6551</v>
       </c>
-      <c r="J299" s="3">
-        <v>12.9</v>
+      <c r="J299" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="K299" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L299" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-12.9</v>
+        <v>--12.9</v>
       </c>
       <c r="M299" s="3">
         <v>20.5</v>
@@ -29003,15 +29285,15 @@
       <c r="D300" s="3">
         <v>230.2</v>
       </c>
-      <c r="E300" s="3">
-        <v>11</v>
+      <c r="E300" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="F300" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G300" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-11</v>
+        <v>--11</v>
       </c>
       <c r="H300" s="3">
         <v>161.4</v>
@@ -29032,15 +29314,15 @@
       <c r="M300" s="3">
         <v>18.399999999999999</v>
       </c>
-      <c r="N300" s="3">
-        <v>7.1</v>
+      <c r="N300" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="O300" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P300" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-7.1</v>
+        <v>--7.1</v>
       </c>
       <c r="Q300" s="3">
         <v>8.4</v>
@@ -29292,15 +29574,15 @@
       <c r="D303" s="3">
         <v>155</v>
       </c>
-      <c r="E303" s="3">
-        <v>12.5</v>
+      <c r="E303" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="F303" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G303" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-12.5</v>
+        <v>--12.5</v>
       </c>
       <c r="H303" s="3">
         <v>111.4</v>
@@ -29308,28 +29590,28 @@
       <c r="I303" s="3">
         <v>5931</v>
       </c>
-      <c r="J303" s="3">
-        <v>12.9</v>
+      <c r="J303" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="K303" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L303" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-12.9</v>
+        <v>--12.9</v>
       </c>
       <c r="M303" s="3">
         <v>20.5</v>
       </c>
-      <c r="N303" s="3">
-        <v>1.4</v>
+      <c r="N303" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O303" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P303" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q303" s="3">
         <v>6</v>
@@ -29389,15 +29671,15 @@
       <c r="D304" s="3">
         <v>218.9</v>
       </c>
-      <c r="E304" s="3">
-        <v>38.6</v>
+      <c r="E304" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="F304" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G304" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-38.6</v>
+        <v>--38.6</v>
       </c>
       <c r="H304" s="3">
         <v>135.69999999999999</v>
@@ -29405,28 +29687,28 @@
       <c r="I304" s="3">
         <v>3241</v>
       </c>
-      <c r="J304" s="3">
-        <v>2.1</v>
+      <c r="J304" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="K304" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L304" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-2.1</v>
+        <v>--2.1</v>
       </c>
       <c r="M304" s="3">
         <v>15.3</v>
       </c>
-      <c r="N304" s="3">
-        <v>10</v>
+      <c r="N304" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O304" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P304" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q304" s="3">
         <v>6.4</v>
@@ -29486,15 +29768,15 @@
       <c r="D305" s="3">
         <v>282.2</v>
       </c>
-      <c r="E305" s="3">
-        <v>41.2</v>
+      <c r="E305" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="F305" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G305" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-41.2</v>
+        <v>--41.2</v>
       </c>
       <c r="H305" s="3">
         <v>165.7</v>
@@ -29513,15 +29795,15 @@
       <c r="M305" s="3">
         <v>16.3</v>
       </c>
-      <c r="N305" s="3">
-        <v>8.6</v>
+      <c r="N305" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O305" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P305" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q305" s="3">
         <v>7.8</v>
@@ -29581,15 +29863,15 @@
       <c r="D306" s="3">
         <v>209</v>
       </c>
-      <c r="E306" s="3">
-        <v>0.5</v>
+      <c r="E306" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="F306" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G306" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-0.5</v>
+        <v>--0.5</v>
       </c>
       <c r="H306" s="3">
         <v>157.1</v>
@@ -29597,15 +29879,15 @@
       <c r="I306" s="3">
         <v>6965</v>
       </c>
-      <c r="J306" s="3">
-        <v>8.6</v>
+      <c r="J306" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="K306" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L306" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="M306" s="3">
         <v>25.8</v>
@@ -29775,15 +30057,15 @@
       <c r="D308" s="3">
         <v>247.4</v>
       </c>
-      <c r="E308" s="3">
-        <v>25.4</v>
+      <c r="E308" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="F308" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G308" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-25.4</v>
+        <v>--25.4</v>
       </c>
       <c r="H308" s="3">
         <v>152.9</v>
@@ -29791,28 +30073,28 @@
       <c r="I308" s="3">
         <v>3655</v>
       </c>
-      <c r="J308" s="3">
-        <v>6.4</v>
+      <c r="J308" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K308" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L308" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M308" s="3">
         <v>18.399999999999999</v>
       </c>
-      <c r="N308" s="3">
-        <v>4.3</v>
+      <c r="N308" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O308" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P308" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q308" s="3">
         <v>7.8</v>
@@ -29872,15 +30154,15 @@
       <c r="D309" s="3">
         <v>248.3</v>
       </c>
-      <c r="E309" s="3">
-        <v>4.9000000000000004</v>
+      <c r="E309" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="F309" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G309" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-4.9</v>
+        <v>--4.9</v>
       </c>
       <c r="H309" s="3">
         <v>178.6</v>
@@ -29901,15 +30183,15 @@
       <c r="M309" s="3">
         <v>22.6</v>
       </c>
-      <c r="N309" s="3">
-        <v>5.7</v>
+      <c r="N309" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="O309" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P309" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-5.7</v>
+        <v>--5.7</v>
       </c>
       <c r="Q309" s="3">
         <v>9.5</v>
@@ -29969,15 +30251,15 @@
       <c r="D310" s="3">
         <v>288.10000000000002</v>
       </c>
-      <c r="E310" s="3">
-        <v>14.4</v>
+      <c r="E310" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="F310" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G310" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-14.4</v>
+        <v>--14.4</v>
       </c>
       <c r="H310" s="3">
         <v>171.4</v>
@@ -29996,15 +30278,15 @@
       <c r="M310" s="3">
         <v>24.7</v>
       </c>
-      <c r="N310" s="3">
-        <v>2.9</v>
+      <c r="N310" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O310" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P310" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q310" s="3">
         <v>9.1</v>
@@ -30064,15 +30346,15 @@
       <c r="D311" s="3">
         <v>296.60000000000002</v>
       </c>
-      <c r="E311" s="3">
-        <v>26.3</v>
+      <c r="E311" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="F311" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G311" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-26.3</v>
+        <v>--26.3</v>
       </c>
       <c r="H311" s="3">
         <v>180</v>
@@ -30093,15 +30375,15 @@
       <c r="M311" s="3">
         <v>13.2</v>
       </c>
-      <c r="N311" s="3">
-        <v>8.6</v>
+      <c r="N311" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O311" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P311" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q311" s="3">
         <v>8.1</v>
@@ -30268,15 +30550,15 @@
       <c r="I313" s="3">
         <v>3862</v>
       </c>
-      <c r="J313" s="3">
-        <v>6.4</v>
+      <c r="J313" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K313" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L313" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M313" s="3">
         <v>22.6</v>
@@ -30446,15 +30728,15 @@
       <c r="D315" s="3">
         <v>217</v>
       </c>
-      <c r="E315" s="3">
-        <v>44.1</v>
+      <c r="E315" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="F315" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G315" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-44.1</v>
+        <v>--44.1</v>
       </c>
       <c r="H315" s="3">
         <v>150</v>
@@ -30462,28 +30744,28 @@
       <c r="I315" s="3">
         <v>4896</v>
       </c>
-      <c r="J315" s="3">
-        <v>15</v>
+      <c r="J315" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="K315" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L315" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-15</v>
+        <v>--15</v>
       </c>
       <c r="M315" s="3">
         <v>26.8</v>
       </c>
-      <c r="N315" s="3">
-        <v>7.1</v>
+      <c r="N315" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="O315" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P315" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-7.1</v>
+        <v>--7.1</v>
       </c>
       <c r="Q315" s="3">
         <v>8.6</v>
@@ -30543,15 +30825,15 @@
       <c r="D316" s="3">
         <v>236.8</v>
       </c>
-      <c r="E316" s="3">
-        <v>28.5</v>
+      <c r="E316" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="F316" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G316" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-28.5</v>
+        <v>--28.5</v>
       </c>
       <c r="H316" s="3">
         <v>154.30000000000001</v>
@@ -30572,15 +30854,15 @@
       <c r="M316" s="3">
         <v>11.1</v>
       </c>
-      <c r="N316" s="3">
-        <v>10</v>
+      <c r="N316" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O316" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P316" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q316" s="3">
         <v>7.1</v>
@@ -31212,15 +31494,15 @@
       <c r="D323" s="3">
         <v>243.4</v>
       </c>
-      <c r="E323" s="3">
-        <v>36.700000000000003</v>
+      <c r="E323" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="F323" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G323" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-36.7</v>
+        <v>--36.7</v>
       </c>
       <c r="H323" s="3">
         <v>157.1</v>
@@ -31241,15 +31523,15 @@
       <c r="M323" s="3">
         <v>13.2</v>
       </c>
-      <c r="N323" s="3">
-        <v>10</v>
+      <c r="N323" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O323" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P323" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q323" s="3">
         <v>7.5</v>
@@ -31309,15 +31591,15 @@
       <c r="D324" s="3">
         <v>214.5</v>
       </c>
-      <c r="E324" s="3">
-        <v>15.6</v>
+      <c r="E324" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="F324" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G324" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-15.6</v>
+        <v>--15.6</v>
       </c>
       <c r="H324" s="3">
         <v>128.6</v>
@@ -31336,15 +31618,15 @@
       <c r="M324" s="3">
         <v>24.7</v>
       </c>
-      <c r="N324" s="3">
-        <v>4.3</v>
+      <c r="N324" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O324" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P324" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q324" s="3">
         <v>7</v>
@@ -31404,15 +31686,15 @@
       <c r="D325" s="3">
         <v>176.7</v>
       </c>
-      <c r="E325" s="3">
-        <v>0.9</v>
+      <c r="E325" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="F325" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G325" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-0.9</v>
+        <v>--0.9</v>
       </c>
       <c r="H325" s="3">
         <v>120</v>
@@ -31433,15 +31715,15 @@
       <c r="M325" s="3">
         <v>26.8</v>
       </c>
-      <c r="N325" s="3">
-        <v>1.4</v>
+      <c r="N325" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O325" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P325" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q325" s="3">
         <v>7</v>
@@ -31501,15 +31783,15 @@
       <c r="D326" s="3">
         <v>197</v>
       </c>
-      <c r="E326" s="3">
-        <v>4.8</v>
+      <c r="E326" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="F326" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G326" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-4.8</v>
+        <v>--4.8</v>
       </c>
       <c r="H326" s="3">
         <v>137.1</v>
@@ -31528,15 +31810,15 @@
       <c r="M326" s="3">
         <v>20.5</v>
       </c>
-      <c r="N326" s="3">
-        <v>1.4</v>
+      <c r="N326" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O326" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P326" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q326" s="3">
         <v>7.5</v>
@@ -31982,15 +32264,15 @@
       <c r="D331" s="3">
         <v>199.5</v>
       </c>
-      <c r="E331" s="3">
-        <v>28</v>
+      <c r="E331" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="F331" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G331" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-28</v>
+        <v>--28</v>
       </c>
       <c r="H331" s="3">
         <v>130</v>
@@ -31998,28 +32280,28 @@
       <c r="I331" s="3">
         <v>3448</v>
       </c>
-      <c r="J331" s="3">
-        <v>4.3</v>
+      <c r="J331" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="K331" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L331" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="M331" s="3">
         <v>26.8</v>
       </c>
-      <c r="N331" s="3">
-        <v>7.1</v>
+      <c r="N331" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="O331" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P331" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-7.1</v>
+        <v>--7.1</v>
       </c>
       <c r="Q331" s="3">
         <v>7.6</v>
@@ -32079,15 +32361,15 @@
       <c r="D332" s="3">
         <v>238.2</v>
       </c>
-      <c r="E332" s="3">
-        <v>12</v>
+      <c r="E332" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="F332" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G332" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-12</v>
+        <v>--12</v>
       </c>
       <c r="H332" s="3">
         <v>165.7</v>
@@ -32106,15 +32388,15 @@
       <c r="M332" s="3">
         <v>20.5</v>
       </c>
-      <c r="N332" s="3">
-        <v>2.9</v>
+      <c r="N332" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O332" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P332" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q332" s="3">
         <v>8.8000000000000007</v>
@@ -32174,15 +32456,15 @@
       <c r="D333" s="3">
         <v>215.4</v>
       </c>
-      <c r="E333" s="3">
-        <v>6.5</v>
+      <c r="E333" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="F333" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G333" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-6.5</v>
+        <v>--6.5</v>
       </c>
       <c r="H333" s="3">
         <v>144.30000000000001</v>
@@ -32203,15 +32485,15 @@
       <c r="M333" s="3">
         <v>19.5</v>
       </c>
-      <c r="N333" s="3">
-        <v>4.3</v>
+      <c r="N333" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O333" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P333" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q333" s="3">
         <v>7.7</v>
@@ -32287,15 +32569,15 @@
       <c r="I334" s="3">
         <v>3448</v>
       </c>
-      <c r="J334" s="3">
-        <v>12.9</v>
+      <c r="J334" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="K334" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L334" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-12.9</v>
+        <v>--12.9</v>
       </c>
       <c r="M334" s="3">
         <v>18.399999999999999</v>
@@ -32465,15 +32747,15 @@
       <c r="D336" s="3">
         <v>197.7</v>
       </c>
-      <c r="E336" s="3">
-        <v>19.899999999999999</v>
+      <c r="E336" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="F336" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G336" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-19.9</v>
+        <v>--19.9</v>
       </c>
       <c r="H336" s="3">
         <v>144.30000000000001</v>
@@ -32494,15 +32776,15 @@
       <c r="M336" s="3">
         <v>26.8</v>
       </c>
-      <c r="N336" s="3">
-        <v>8.6</v>
+      <c r="N336" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O336" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P336" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q336" s="3">
         <v>8.4</v>
@@ -32754,15 +33036,15 @@
       <c r="D339" s="3">
         <v>186.3</v>
       </c>
-      <c r="E339" s="3">
-        <v>13.7</v>
+      <c r="E339" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="F339" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G339" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-13.7</v>
+        <v>--13.7</v>
       </c>
       <c r="H339" s="3">
         <v>128.6</v>
@@ -32781,15 +33063,15 @@
       <c r="M339" s="3">
         <v>11.1</v>
       </c>
-      <c r="N339" s="3">
-        <v>4.3</v>
+      <c r="N339" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O339" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P339" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q339" s="3">
         <v>5.9</v>
@@ -32849,15 +33131,15 @@
       <c r="D340" s="3">
         <v>156.80000000000001</v>
       </c>
-      <c r="E340" s="3">
-        <v>17.7</v>
+      <c r="E340" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="F340" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G340" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-17.7</v>
+        <v>--17.7</v>
       </c>
       <c r="H340" s="3">
         <v>111.4</v>
@@ -32865,28 +33147,28 @@
       <c r="I340" s="3">
         <v>5310</v>
       </c>
-      <c r="J340" s="3">
-        <v>4.3</v>
+      <c r="J340" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="K340" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L340" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="M340" s="3">
         <v>13.2</v>
       </c>
-      <c r="N340" s="3">
-        <v>5.7</v>
+      <c r="N340" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="O340" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P340" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-5.7</v>
+        <v>--5.7</v>
       </c>
       <c r="Q340" s="3">
         <v>5.2</v>
@@ -33041,15 +33323,15 @@
       <c r="D342" s="3">
         <v>174</v>
       </c>
-      <c r="E342" s="3">
-        <v>11.7</v>
+      <c r="E342" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="F342" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G342" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-11.7</v>
+        <v>--11.7</v>
       </c>
       <c r="H342" s="3">
         <v>120</v>
@@ -33057,15 +33339,15 @@
       <c r="I342" s="3">
         <v>4275</v>
       </c>
-      <c r="J342" s="3">
-        <v>15</v>
+      <c r="J342" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="K342" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L342" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-15</v>
+        <v>--15</v>
       </c>
       <c r="M342" s="3">
         <v>27.9</v>
@@ -33136,15 +33418,15 @@
       <c r="D343" s="3">
         <v>181</v>
       </c>
-      <c r="E343" s="3">
-        <v>26.5</v>
+      <c r="E343" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="F343" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G343" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-26.5</v>
+        <v>--26.5</v>
       </c>
       <c r="H343" s="3">
         <v>118.6</v>
@@ -33152,28 +33434,28 @@
       <c r="I343" s="3">
         <v>3448</v>
       </c>
-      <c r="J343" s="3">
-        <v>6.4</v>
+      <c r="J343" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K343" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L343" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M343" s="3">
         <v>25.8</v>
       </c>
-      <c r="N343" s="3">
-        <v>7.1</v>
+      <c r="N343" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="O343" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P343" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-7.1</v>
+        <v>--7.1</v>
       </c>
       <c r="Q343" s="3">
         <v>6.8</v>
@@ -33233,15 +33515,15 @@
       <c r="D344" s="3">
         <v>220.4</v>
       </c>
-      <c r="E344" s="3">
-        <v>6</v>
+      <c r="E344" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F344" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G344" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-6</v>
+        <v>--6</v>
       </c>
       <c r="H344" s="3">
         <v>150</v>
@@ -33262,15 +33544,15 @@
       <c r="M344" s="3">
         <v>24.7</v>
       </c>
-      <c r="N344" s="3">
-        <v>2.9</v>
+      <c r="N344" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O344" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P344" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q344" s="3">
         <v>8.5</v>
@@ -33330,15 +33612,15 @@
       <c r="D345" s="3">
         <v>216.3</v>
       </c>
-      <c r="E345" s="3">
-        <v>25.9</v>
+      <c r="E345" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="F345" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G345" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-25.9</v>
+        <v>--25.9</v>
       </c>
       <c r="H345" s="3">
         <v>144.30000000000001</v>
@@ -33346,28 +33628,28 @@
       <c r="I345" s="3">
         <v>4068</v>
       </c>
-      <c r="J345" s="3">
-        <v>4.3</v>
+      <c r="J345" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="K345" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L345" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="M345" s="3">
         <v>26.8</v>
       </c>
-      <c r="N345" s="3">
-        <v>5.7</v>
+      <c r="N345" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="O345" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P345" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-5.7</v>
+        <v>--5.7</v>
       </c>
       <c r="Q345" s="3">
         <v>8.3000000000000007</v>
@@ -33522,15 +33804,15 @@
       <c r="D347" s="3">
         <v>262.8</v>
       </c>
-      <c r="E347" s="3">
-        <v>19.3</v>
+      <c r="E347" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="F347" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G347" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-19.3</v>
+        <v>--19.3</v>
       </c>
       <c r="H347" s="3">
         <v>155.69999999999999</v>
@@ -33549,15 +33831,15 @@
       <c r="M347" s="3">
         <v>19.5</v>
       </c>
-      <c r="N347" s="3">
-        <v>4.3</v>
+      <c r="N347" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O347" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P347" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q347" s="3">
         <v>7.9</v>
@@ -33617,15 +33899,15 @@
       <c r="D348" s="3">
         <v>192.7</v>
       </c>
-      <c r="E348" s="3">
-        <v>3.3</v>
+      <c r="E348" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F348" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G348" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-3.3</v>
+        <v>--3.3</v>
       </c>
       <c r="H348" s="3">
         <v>157.1</v>
@@ -33633,15 +33915,15 @@
       <c r="I348" s="3">
         <v>7586</v>
       </c>
-      <c r="J348" s="3">
-        <v>6.4</v>
+      <c r="J348" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K348" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L348" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M348" s="3">
         <v>30</v>
@@ -33714,15 +33996,15 @@
       <c r="D349" s="3">
         <v>275.8</v>
       </c>
-      <c r="E349" s="3">
-        <v>31.9</v>
+      <c r="E349" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="F349" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G349" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-31.9</v>
+        <v>--31.9</v>
       </c>
       <c r="H349" s="3">
         <v>174.3</v>
@@ -33743,15 +34025,15 @@
       <c r="M349" s="3">
         <v>15.3</v>
       </c>
-      <c r="N349" s="3">
-        <v>8.6</v>
+      <c r="N349" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O349" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P349" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q349" s="3">
         <v>8.4</v>
@@ -33811,15 +34093,15 @@
       <c r="D350" s="3">
         <v>176.4</v>
       </c>
-      <c r="E350" s="3">
-        <v>2.6</v>
+      <c r="E350" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="F350" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G350" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-2.6</v>
+        <v>--2.6</v>
       </c>
       <c r="H350" s="3">
         <v>114.3</v>
@@ -33840,15 +34122,15 @@
       <c r="M350" s="3">
         <v>16.3</v>
       </c>
-      <c r="N350" s="3">
-        <v>2.9</v>
+      <c r="N350" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O350" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P350" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q350" s="3">
         <v>5.3</v>
@@ -33908,15 +34190,15 @@
       <c r="D351" s="3">
         <v>203.1</v>
       </c>
-      <c r="E351" s="3">
-        <v>28</v>
+      <c r="E351" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="F351" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G351" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-28</v>
+        <v>--28</v>
       </c>
       <c r="H351" s="3">
         <v>130</v>
@@ -33937,15 +34219,15 @@
       <c r="M351" s="3">
         <v>18.399999999999999</v>
       </c>
-      <c r="N351" s="3">
-        <v>8.6</v>
+      <c r="N351" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O351" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P351" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q351" s="3">
         <v>6.7</v>
@@ -34021,15 +34303,15 @@
       <c r="I352" s="3">
         <v>7172</v>
       </c>
-      <c r="J352" s="3">
-        <v>4.3</v>
+      <c r="J352" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="K352" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L352" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="M352" s="3">
         <v>24.7</v>
@@ -34292,15 +34574,15 @@
       <c r="D355" s="3">
         <v>188.6</v>
       </c>
-      <c r="E355" s="3">
-        <v>9.4</v>
+      <c r="E355" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="F355" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G355" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-9.4</v>
+        <v>--9.4</v>
       </c>
       <c r="H355" s="3">
         <v>127.1</v>
@@ -34319,15 +34601,15 @@
       <c r="M355" s="3">
         <v>17.399999999999999</v>
       </c>
-      <c r="N355" s="3">
-        <v>2.9</v>
+      <c r="N355" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O355" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P355" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q355" s="3">
         <v>6.6</v>
@@ -34500,15 +34782,15 @@
       <c r="I357" s="3">
         <v>3862</v>
       </c>
-      <c r="J357" s="3">
-        <v>10.7</v>
+      <c r="J357" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K357" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L357" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-10.7</v>
+        <v>--10.7</v>
       </c>
       <c r="M357" s="3">
         <v>26.8</v>
@@ -34597,15 +34879,15 @@
       <c r="I358" s="3">
         <v>2827</v>
       </c>
-      <c r="J358" s="3">
-        <v>8.6</v>
+      <c r="J358" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="K358" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L358" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="M358" s="3">
         <v>10</v>
@@ -34789,15 +35071,15 @@
       <c r="I360" s="3">
         <v>5724</v>
       </c>
-      <c r="J360" s="3">
-        <v>12.9</v>
+      <c r="J360" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="K360" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L360" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-12.9</v>
+        <v>--12.9</v>
       </c>
       <c r="M360" s="3">
         <v>22.6</v>
@@ -34994,15 +35276,15 @@
       <c r="M362" s="3">
         <v>18.399999999999999</v>
       </c>
-      <c r="N362" s="3">
-        <v>1.4</v>
+      <c r="N362" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O362" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P362" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q362" s="3">
         <v>7.4</v>
@@ -35188,15 +35470,15 @@
       <c r="M364" s="3">
         <v>22.6</v>
       </c>
-      <c r="N364" s="3">
-        <v>1.4</v>
+      <c r="N364" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="O364" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P364" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-1.4</v>
+        <v>--1.4</v>
       </c>
       <c r="Q364" s="3">
         <v>9.3000000000000007</v>
@@ -35369,15 +35651,15 @@
       <c r="I366" s="3">
         <v>2827</v>
       </c>
-      <c r="J366" s="3">
-        <v>6.4</v>
+      <c r="J366" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K366" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L366" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M366" s="3">
         <v>26.8</v>
@@ -35450,15 +35732,15 @@
       <c r="D367" s="3">
         <v>186.6</v>
       </c>
-      <c r="E367" s="3">
-        <v>31.9</v>
+      <c r="E367" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="F367" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G367" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-31.9</v>
+        <v>--31.9</v>
       </c>
       <c r="H367" s="3">
         <v>125.7</v>
@@ -35477,15 +35759,15 @@
       <c r="M367" s="3">
         <v>23.7</v>
       </c>
-      <c r="N367" s="3">
-        <v>10</v>
+      <c r="N367" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O367" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P367" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q367" s="3">
         <v>7.1</v>
@@ -35561,15 +35843,15 @@
       <c r="I368" s="3">
         <v>6551</v>
       </c>
-      <c r="J368" s="3">
-        <v>8.6</v>
+      <c r="J368" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="K368" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L368" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="M368" s="3">
         <v>14.2</v>
@@ -35850,15 +36132,15 @@
       <c r="I371" s="3">
         <v>8000</v>
       </c>
-      <c r="J371" s="3">
-        <v>6.4</v>
+      <c r="J371" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="K371" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L371" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-6.4</v>
+        <v>--6.4</v>
       </c>
       <c r="M371" s="3">
         <v>13.2</v>
@@ -35931,15 +36213,15 @@
       <c r="D372" s="3">
         <v>268.89999999999998</v>
       </c>
-      <c r="E372" s="3">
-        <v>12.6</v>
+      <c r="E372" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="F372" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G372" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-12.6</v>
+        <v>--12.6</v>
       </c>
       <c r="H372" s="3">
         <v>162.9</v>
@@ -35947,15 +36229,15 @@
       <c r="I372" s="3">
         <v>2827</v>
       </c>
-      <c r="J372" s="3">
-        <v>12.9</v>
+      <c r="J372" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="K372" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L372" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-12.9</v>
+        <v>--12.9</v>
       </c>
       <c r="M372" s="3">
         <v>10</v>
@@ -36121,15 +36403,15 @@
       <c r="D374" s="3">
         <v>255.9</v>
       </c>
-      <c r="E374" s="3">
-        <v>12.3</v>
+      <c r="E374" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="F374" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G374" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-12.3</v>
+        <v>--12.3</v>
       </c>
       <c r="H374" s="3">
         <v>171.4</v>
@@ -36137,15 +36419,15 @@
       <c r="I374" s="3">
         <v>6137</v>
       </c>
-      <c r="J374" s="3">
-        <v>8.6</v>
+      <c r="J374" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="K374" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L374" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="M374" s="3">
         <v>16.3</v>
@@ -36216,15 +36498,15 @@
       <c r="D375" s="3">
         <v>183.7</v>
       </c>
-      <c r="E375" s="3">
-        <v>36.9</v>
+      <c r="E375" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="F375" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G375" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-36.9</v>
+        <v>--36.9</v>
       </c>
       <c r="H375" s="3">
         <v>141.4</v>
@@ -36232,28 +36514,28 @@
       <c r="I375" s="3">
         <v>7793</v>
       </c>
-      <c r="J375" s="3">
-        <v>12.9</v>
+      <c r="J375" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="K375" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L375" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-12.9</v>
+        <v>--12.9</v>
       </c>
       <c r="M375" s="3">
         <v>24.7</v>
       </c>
-      <c r="N375" s="3">
-        <v>7.1</v>
+      <c r="N375" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="O375" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P375" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-7.1</v>
+        <v>--7.1</v>
       </c>
       <c r="Q375" s="3">
         <v>8</v>
@@ -36313,15 +36595,15 @@
       <c r="D376" s="3">
         <v>279</v>
       </c>
-      <c r="E376" s="3">
-        <v>8.6</v>
+      <c r="E376" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="F376" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G376" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="H376" s="3">
         <v>178.6</v>
@@ -36342,15 +36624,15 @@
       <c r="M376" s="3">
         <v>11.1</v>
       </c>
-      <c r="N376" s="3">
-        <v>4.3</v>
+      <c r="N376" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O376" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P376" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q376" s="3">
         <v>8</v>
@@ -36410,15 +36692,15 @@
       <c r="D377" s="3">
         <v>190.9</v>
       </c>
-      <c r="E377" s="3">
-        <v>7.6</v>
+      <c r="E377" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="F377" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G377" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-7.6</v>
+        <v>--7.6</v>
       </c>
       <c r="H377" s="3">
         <v>134.30000000000001</v>
@@ -36439,15 +36721,15 @@
       <c r="M377" s="3">
         <v>11.1</v>
       </c>
-      <c r="N377" s="3">
-        <v>2.9</v>
+      <c r="N377" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O377" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P377" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q377" s="3">
         <v>6.3</v>
@@ -36507,15 +36789,15 @@
       <c r="D378" s="3">
         <v>165.4</v>
       </c>
-      <c r="E378" s="3">
-        <v>30.4</v>
+      <c r="E378" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="F378" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G378" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-30.4</v>
+        <v>--30.4</v>
       </c>
       <c r="H378" s="3">
         <v>112.9</v>
@@ -36523,28 +36805,28 @@
       <c r="I378" s="3">
         <v>3241</v>
       </c>
-      <c r="J378" s="3">
-        <v>8.6</v>
+      <c r="J378" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="K378" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L378" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="M378" s="3">
         <v>11.1</v>
       </c>
-      <c r="N378" s="3">
-        <v>10</v>
+      <c r="N378" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O378" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P378" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q378" s="3">
         <v>4.5</v>
@@ -36701,15 +36983,15 @@
       <c r="D380" s="3">
         <v>149</v>
       </c>
-      <c r="E380" s="3">
-        <v>22.1</v>
+      <c r="E380" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="F380" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G380" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-22.1</v>
+        <v>--22.1</v>
       </c>
       <c r="H380" s="3">
         <v>110</v>
@@ -36728,15 +37010,15 @@
       <c r="M380" s="3">
         <v>21.6</v>
       </c>
-      <c r="N380" s="3">
-        <v>8.6</v>
+      <c r="N380" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O380" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P380" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q380" s="3">
         <v>6.1</v>
@@ -36796,15 +37078,15 @@
       <c r="D381" s="3">
         <v>245</v>
       </c>
-      <c r="E381" s="3">
-        <v>57.9</v>
+      <c r="E381" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="F381" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G381" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-57.9</v>
+        <v>--57.9</v>
       </c>
       <c r="H381" s="3">
         <v>171.4</v>
@@ -36812,28 +37094,28 @@
       <c r="I381" s="3">
         <v>7793</v>
       </c>
-      <c r="J381" s="3">
-        <v>15</v>
+      <c r="J381" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="K381" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L381" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-15</v>
+        <v>--15</v>
       </c>
       <c r="M381" s="3">
         <v>14.2</v>
       </c>
-      <c r="N381" s="3">
-        <v>8.6</v>
+      <c r="N381" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="O381" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P381" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-8.6</v>
+        <v>--8.6</v>
       </c>
       <c r="Q381" s="3">
         <v>8.3000000000000007</v>
@@ -37017,15 +37299,15 @@
       <c r="M383" s="3">
         <v>20.5</v>
       </c>
-      <c r="N383" s="3">
-        <v>4.3</v>
+      <c r="N383" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O383" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P383" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q383" s="3">
         <v>7.1</v>
@@ -37085,15 +37367,15 @@
       <c r="D384" s="3">
         <v>194</v>
       </c>
-      <c r="E384" s="3">
-        <v>8</v>
+      <c r="E384" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="F384" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G384" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-8</v>
+        <v>--8</v>
       </c>
       <c r="H384" s="3">
         <v>135.69999999999999</v>
@@ -37114,15 +37396,15 @@
       <c r="M384" s="3">
         <v>18.399999999999999</v>
       </c>
-      <c r="N384" s="3">
-        <v>4.3</v>
+      <c r="N384" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="O384" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P384" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-4.3</v>
+        <v>--4.3</v>
       </c>
       <c r="Q384" s="3">
         <v>7.2</v>
@@ -37182,15 +37464,15 @@
       <c r="D385" s="3">
         <v>231.6</v>
       </c>
-      <c r="E385" s="3">
-        <v>50.5</v>
+      <c r="E385" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="F385" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G385" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-50.5</v>
+        <v>--50.5</v>
       </c>
       <c r="H385" s="3">
         <v>140</v>
@@ -37198,28 +37480,28 @@
       <c r="I385" s="3">
         <v>2827</v>
       </c>
-      <c r="J385" s="3">
-        <v>12.9</v>
+      <c r="J385" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="K385" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L385" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-12.9</v>
+        <v>--12.9</v>
       </c>
       <c r="M385" s="3">
         <v>18.399999999999999</v>
       </c>
-      <c r="N385" s="3">
-        <v>10</v>
+      <c r="N385" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="O385" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P385" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-10</v>
+        <v>--10</v>
       </c>
       <c r="Q385" s="3">
         <v>7</v>
@@ -37295,15 +37577,15 @@
       <c r="I386" s="3">
         <v>7379</v>
       </c>
-      <c r="J386" s="3">
-        <v>2.1</v>
+      <c r="J386" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="K386" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L386" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-2.1</v>
+        <v>--2.1</v>
       </c>
       <c r="M386" s="3">
         <v>11.1</v>
@@ -37376,15 +37658,15 @@
       <c r="D387" s="3">
         <v>214.4</v>
       </c>
-      <c r="E387" s="3">
-        <v>24</v>
+      <c r="E387" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="F387" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G387" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column1]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Lateral (yd)]]),Table1[[#This Row],[Lateral (yd)]])</f>
-        <v>-24</v>
+        <v>--24</v>
       </c>
       <c r="H387" s="3">
         <v>154.30000000000001</v>
@@ -37392,28 +37674,28 @@
       <c r="I387" s="3">
         <v>5724</v>
       </c>
-      <c r="J387" s="3">
-        <v>10.7</v>
+      <c r="J387" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K387" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L387" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column2]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Spin Axis (deg)]]),Table1[[#This Row],[Spin Axis (deg)]])</f>
-        <v>-10.7</v>
+        <v>--10.7</v>
       </c>
       <c r="M387" s="3">
         <v>26.8</v>
       </c>
-      <c r="N387" s="3">
-        <v>2.9</v>
+      <c r="N387" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="O387" s="4" t="s">
         <v>22</v>
       </c>
       <c r="P387" s="1" t="str">
         <f>IF(Table1[[#This Row],[Column3]]="L",_xlfn.CONCAT("-",Table1[[#This Row],[Launch H (deg)]]),Table1[[#This Row],[Launch H (deg)]])</f>
-        <v>-2.9</v>
+        <v>--2.9</v>
       </c>
       <c r="Q387" s="3">
         <v>8.8000000000000007</v>

</xml_diff>